<commit_message>
:tada: various updates following review with IDC
</commit_message>
<xml_diff>
--- a/sourceFile/Final IDC Insights DX Taxonomies_3-29-18.xlsx
+++ b/sourceFile/Final IDC Insights DX Taxonomies_3-29-18.xlsx
@@ -9405,6 +9405,7 @@
     <xf numFmtId="2" fontId="24" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9417,7 +9418,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_ 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -10369,7 +10369,7 @@
         <f>A16+1</f>
         <v>14</v>
       </c>
-      <c r="B17" s="124" t="s">
+      <c r="B17" s="120" t="s">
         <v>2685</v>
       </c>
       <c r="C17" t="s">
@@ -10396,7 +10396,7 @@
     </row>
     <row r="18" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="124" t="s">
+      <c r="B18" s="120" t="s">
         <v>2686</v>
       </c>
       <c r="C18" s="74" t="s">
@@ -10553,11 +10553,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -11771,11 +11771,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -12902,11 +12902,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -13861,11 +13861,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="22">
@@ -14706,11 +14706,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="22">
@@ -17713,11 +17713,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -19076,11 +19076,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -20466,11 +20466,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="3"/>
@@ -21728,11 +21728,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="3"/>
@@ -23025,11 +23025,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="4" spans="1:34" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
@@ -46466,11 +46466,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -47423,11 +47423,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -48045,7 +48045,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48063,11 +48063,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="22">
@@ -49339,11 +49339,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -50295,11 +50295,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -51339,11 +51339,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">
@@ -52471,11 +52471,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="4">

</xml_diff>